<commit_message>
Add new PACIO code system and value set
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pacio-cs.xlsx
+++ b/output/StructureDefinition-pacio-cs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="411">
   <si>
     <t>Path</t>
   </si>
@@ -533,7 +533,7 @@
 </t>
   </si>
   <si>
-    <t>Classification of  type of observation</t>
+    <t>A second category code may be used along with the code “functioning”. For example, for assessment tool/survey instrument observations use “survey” as a second code.</t>
   </si>
   <si>
     <t>A code that classifies the general type of observation being made.</t>
@@ -545,10 +545,18 @@
     <t>Used for filtering what observations are retrieved and displayed.</t>
   </si>
   <si>
-    <t>Codes for high level observation categories.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-category</t>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://paciowg.github.io/cognitive-status-ig/CodeSystem/pacio-cat-cs"/&gt;
+    &lt;code value="functioning"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>http://paciowg.github.io/cognitive-status-ig/ValueSet/pacio-cat-vs</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode="COMP].target[classCode="LIST", moodCode="EVN"].code</t>
@@ -574,9 +582,6 @@
   </si>
   <si>
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
-  </si>
-  <si>
-    <t>extensible</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
@@ -1488,7 +1493,7 @@
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.40625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="61.140625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
@@ -3270,7 +3275,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>162</v>
       </c>
@@ -3280,13 +3285,13 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>44</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>45</v>
@@ -3317,7 +3322,7 @@
         <v>45</v>
       </c>
       <c r="R16" t="s" s="2">
-        <v>45</v>
+        <v>168</v>
       </c>
       <c r="S16" t="s" s="2">
         <v>45</v>
@@ -3332,13 +3337,11 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="X16" t="s" s="2">
-        <v>168</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="X16" s="2"/>
       <c r="Y16" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3380,10 +3383,10 @@
         <v>45</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3391,11 +3394,11 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3417,16 +3420,16 @@
         <v>163</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3451,7 +3454,7 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" t="s" s="2">
@@ -3473,7 +3476,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>55</v>
@@ -4395,7 +4398,7 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="X25" t="s" s="2">
         <v>255</v>
@@ -4514,7 +4517,7 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="X26" t="s" s="2">
         <v>264</v>
@@ -7071,7 +7074,7 @@
         <v>396</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7096,7 +7099,7 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" t="s" s="2">
@@ -7332,7 +7335,7 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="X50" t="s" s="2">
         <v>255</v>
@@ -7451,7 +7454,7 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="X51" t="s" s="2">
         <v>264</v>

</xml_diff>